<commit_message>
CHanged from npuj to chg pwd
</commit_message>
<xml_diff>
--- a/data/Playlist.xlsx
+++ b/data/Playlist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sreedevi.pratap\eclipse-workspace\KYC2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sreedevi.pratap\eclipse-workspace\MyTest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820E77EA-25BA-4726-99C7-A9AC9F4339EB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D168FF8E-15AE-4834-9AC5-0D9DBC87D9F6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" tabRatio="918" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -654,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J75" sqref="J75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1409,7 +1409,7 @@
         <v>72</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>